<commit_message>
Update BOM: added link to Schneider LMDCM851 new constructor Novanta IMS
</commit_message>
<xml_diff>
--- a/docs/pySAS.BOM.xlsx
+++ b/docs/pySAS.BOM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils/Documents/Lab/MyPapers/PaperPySAS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils/PycharmProjects/pySAS/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC24844-FCE2-0640-9B2A-0E1AADBA2BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5086E914-489E-C041-A87F-55A1DE29BB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41160" yWindow="2440" windowWidth="27640" windowHeight="16940" xr2:uid="{8954B77B-AA51-5E4D-A126-96B217D1D53D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
   <si>
     <t>Tower</t>
   </si>
@@ -353,6 +353,9 @@
   </si>
   <si>
     <t>Rotary Shaft Seal</t>
+  </si>
+  <si>
+    <t>https://novantaims.com/liberty-mdrives/lh85-nema-34-programmable-motion-control-ip20-lmom85/</t>
   </si>
 </sst>
 </file>
@@ -889,8 +892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB30D09-70ED-6E46-895F-ABAD0978A38E}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1517,6 +1520,9 @@
       </c>
       <c r="C30" t="s">
         <v>92</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>106</v>
       </c>
       <c r="E30">
         <v>1</v>
@@ -1757,6 +1763,7 @@
     <hyperlink ref="D31" r:id="rId30" xr:uid="{63B18B15-B998-CD4F-BF8A-77D78A7812CF}"/>
     <hyperlink ref="D32" r:id="rId31" xr:uid="{07BB656F-215D-4D4B-9F02-B1BB22A78A29}"/>
     <hyperlink ref="D33" r:id="rId32" xr:uid="{24EB6D9A-4514-E341-AB4B-A62D3EAD6F71}"/>
+    <hyperlink ref="D30" r:id="rId33" xr:uid="{783E9EA8-964D-3042-9989-BB5925D36400}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update installation procedure to Raspbian Bookworm.
   - simplified secure thanks to update of OS
   - no need to update hostname anymore
   - hotspot is now handled by nmcli
   - python upgraded to 3.11, more python packages installed with apt
   - use venv for packages not handled by apt
   - use raspi-config read-only mode instead of custom script from adafruit
   - updated requirements.txt
   - migrated plotly code to v6
   - updated BOM
</commit_message>
<xml_diff>
--- a/docs/pySAS.BOM.xlsx
+++ b/docs/pySAS.BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils/PycharmProjects/pySAS/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nils/Documents/Lab/Engineering/pySAS/Quotes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5086E914-489E-C041-A87F-55A1DE29BB3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C49629A-E23E-C842-B6A4-5F91A78C2523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41160" yWindow="2440" windowWidth="27640" windowHeight="16940" xr2:uid="{8954B77B-AA51-5E4D-A126-96B217D1D53D}"/>
+    <workbookView xWindow="84380" yWindow="4200" windowWidth="20180" windowHeight="21900" xr2:uid="{8954B77B-AA51-5E4D-A126-96B217D1D53D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="107">
-  <si>
-    <t>Tower</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="98">
   <si>
     <t>Controller Box</t>
   </si>
@@ -58,15 +56,6 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>Power Supply 220/110V to 12V, 8.5Amps</t>
-  </si>
-  <si>
-    <t>HOTOR 8.5A AC to DC Converter</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/HOTOR-Converter-110-220V-Cigarette-Inflator/dp/B09F2H88KY/r</t>
-  </si>
-  <si>
     <t>Tobsun 50W DC-DC Converter 24/12V to 5V</t>
   </si>
   <si>
@@ -82,18 +71,12 @@
     <t>BONATECH 6 way fuse box</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Warning-Protection-Automotive-Detailed-Instruction/dp/B07M6PLJWF/</t>
-  </si>
-  <si>
     <t>https://www.amazon.com/Blue-Sea-Systems-2315-Terminal/dp/B000OTJ89Q/</t>
   </si>
   <si>
     <t>Raspberry Pi 3B+</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/raspberry-pi/RASPBERRY-PI-3-MODEL-B/8571724</t>
-  </si>
-  <si>
     <t>Heat Sink</t>
   </si>
   <si>
@@ -118,9 +101,6 @@
     <t>https://www.amazon.com/SanDisk-256GB-Ultra-Flash-Drive/dp/B07857Y17V/</t>
   </si>
   <si>
-    <t>ArduSimple KIT009</t>
-  </si>
-  <si>
     <t>https://www.ardusimple.com/product/simplertk2b-heading-basic-starter-kit-ip67/</t>
   </si>
   <si>
@@ -130,18 +110,12 @@
     <t>Gaermo GM-FTDI4X-M</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B01MUDQ6VR/</t>
-  </si>
-  <si>
     <t>4 Channel Relay Module</t>
   </si>
   <si>
     <t>ELEGOO Relay Module 4 Channel</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B01HEQF5HU/</t>
-  </si>
-  <si>
     <t>MicroUSB Type B Cable(Pi)</t>
   </si>
   <si>
@@ -157,9 +131,6 @@
     <t>StarTech USBAB1MR</t>
   </si>
   <si>
-    <t>https://www.startech.com/en-us/cables/usbab1mr</t>
-  </si>
-  <si>
     <t>Passive RS232 to RS485/422 Converter</t>
   </si>
   <si>
@@ -169,24 +140,12 @@
     <t>https://www.amazon.com/gp/product/B0196AO1IG/</t>
   </si>
   <si>
-    <t>RS232 Shifter</t>
-  </si>
-  <si>
-    <t>Sparkfun PRT-00449</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/sparkfun-electronics/PRT-00449/5762433</t>
-  </si>
-  <si>
     <t>RS232 Terminal Block</t>
   </si>
   <si>
     <t>Uxcell DB9-M3-G3</t>
   </si>
   <si>
-    <t>https://www.amazon.com/uxcell-DB9-M3-G3-Position-Terminal-Connector/dp/B01NH5HQ4U/</t>
-  </si>
-  <si>
     <t>Panel mount 3-pin male connector</t>
   </si>
   <si>
@@ -232,39 +191,12 @@
     <t>https://www.mcmaster.com/7152k64/</t>
   </si>
   <si>
-    <t>Panel mount 7-pin male connector</t>
-  </si>
-  <si>
-    <t>McMaster 3216K57</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/3216K57/</t>
-  </si>
-  <si>
-    <t>Cap 7-pin connector</t>
-  </si>
-  <si>
     <t>McMaster 69005K64</t>
   </si>
   <si>
     <t>https://www.mcmaster.com/69005K64/</t>
   </si>
   <si>
-    <t>McMaster 69285K13</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/69285k13/</t>
-  </si>
-  <si>
-    <t>Panel mount 7-pin female connector</t>
-  </si>
-  <si>
-    <t>McMaster 3216K58</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/3216k58/</t>
-  </si>
-  <si>
     <t>50' Power Extension Cord</t>
   </si>
   <si>
@@ -292,9 +224,6 @@
     <t>https://www.mcmaster.com/3762n116/</t>
   </si>
   <si>
-    <t>See drawings</t>
-  </si>
-  <si>
     <t>Pelican 1500 Case</t>
   </si>
   <si>
@@ -307,55 +236,100 @@
     <t>Other (wires, fuses, standoffs)</t>
   </si>
   <si>
-    <t>Cables</t>
-  </si>
-  <si>
     <t>Common Bar</t>
   </si>
   <si>
-    <t>Schneider LMDCM851</t>
-  </si>
-  <si>
-    <t>Precision planetary reduction gearbox</t>
-  </si>
-  <si>
-    <t>Stepper motor</t>
-  </si>
-  <si>
-    <t>PGCN34-5050</t>
-  </si>
-  <si>
-    <t>https://www.automationdirect.com/adc/shopping/catalog/power_transmission_(mechanical)/precision_gearboxes_for_small_nema_motors/nema_34_frame/pgcn34-5050</t>
-  </si>
-  <si>
-    <t>McMaster 5154T94</t>
-  </si>
-  <si>
-    <t>https://www.mcmaster.com/5154T94/</t>
-  </si>
-  <si>
     <t>Blue Sea Systems - 100A - 5 screw with cover</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>Custom stainless-steel parts see drawings</t>
-  </si>
-  <si>
-    <t>Cable 7-pin 6 ft (Controller Box to Tower)</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t>Dual RTK GNSS GPS</t>
   </si>
   <si>
-    <t>Rotary Shaft Seal</t>
-  </si>
-  <si>
-    <t>https://novantaims.com/liberty-mdrives/lh85-nema-34-programmable-motion-control-ip20-lmom85/</t>
+    <t>https://www.amazon.com/Gearmo-Industrial-4-Port-Chipset-Indicators/dp/B08GTQLP81/</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/DB9-M3-G3-RS232-Adapterplatte-Positionen-Klemmenanschlussmodul-Signalmodul/dp/B09GRTMGX4/</t>
+  </si>
+  <si>
+    <t>Check Other Ref</t>
+  </si>
+  <si>
+    <t>Low Stock</t>
+  </si>
+  <si>
+    <t>Tower Connector</t>
+  </si>
+  <si>
+    <t>Cables/Connectors</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/69285K14</t>
+  </si>
+  <si>
+    <t>McMaster 69285K14</t>
+  </si>
+  <si>
+    <t>Cable 8-pin 6 ft (Controller Box to Tower)</t>
+  </si>
+  <si>
+    <t>McMaster 3216K59</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/3216K59/</t>
+  </si>
+  <si>
+    <t>McMaster 3216K61</t>
+  </si>
+  <si>
+    <t>Panel mount 8-pin male connector</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/3216K61/</t>
+  </si>
+  <si>
+    <t>Panel mount 8-pin female connector</t>
+  </si>
+  <si>
+    <t>Cap 8-pin connector</t>
+  </si>
+  <si>
+    <t>ArduSimple AS-ADP-ARDUINO-TO-RPI-00</t>
+  </si>
+  <si>
+    <t>https://www.ardusimple.com/product/raspberry-adapter-for-simplertk2b/</t>
+  </si>
+  <si>
+    <t>RPi Adapter for RTK GPS (free one serial port)</t>
+  </si>
+  <si>
+    <t>Power Supply 220/110V to 12V, 5Amps</t>
+  </si>
+  <si>
+    <t>TracoPower TMPW 50-1120T</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/traco-power/TMPW%252050-112-T/20525617?gclsrc=aw.ds&amp;&amp;utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_ITECH&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21147141757_adg-_ad-__dev-c_ext-_prd-20525617_sig-CjwKCAiA3ZC6BhBaEiwAeqfvyjKG0U8PWJcrc_QQsXyUxfll2yvNX7vfMULlS1uMNy8c9vlZJXY1VxoCGvoQAvD_BwE&amp;gad_source=1&amp;gbraid=0AAAAADrbLljvEBu8WsSuhejydM0PsvfLA&amp;gclid=CjwKCAiA3ZC6BhBaEiwAeqfvyjKG0U8PWJcrc_QQsXyUxfll2yvNX7vfMULlS1uMNy8c9vlZJXY1VxoCGvoQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/Warning-Protection-Automotive-Detailed-Instruction/dp/B08QYZT6ZB/</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/raspberry-pi/SC0073/8571724?gclsrc=aw.ds&amp;&amp;utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=PMax%20Shopping_Product_Medium%20ROAS%20Categories&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-20223376311_adg-_ad-__dev-c_ext-_prd-8571724_sig-CjwKCAiA3ZC6BhBaEiwAeqfvyr1Y3hc13PNC4iBVVwTKge1OTkkkcAgc8lJGj1BlAnGllHXnVnq21BoC1RMQAvD_BwE&amp;gad_source=1&amp;gbraid=0AAAAADrbLlhlVClGpzPjfDAQRmRcbv9RA&amp;gclid=CjwKCAiA3ZC6BhBaEiwAeqfvyr1Y3hc13PNC4iBVVwTKge1OTkkkcAgc8lJGj1BlAnGllHXnVnq21BoC1RMQAvD_BwE&amp;gclsrc=aw.ds</t>
+  </si>
+  <si>
+    <t>ArduSimple AS-STARTKIT-HEAD-L1L2</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/SunFounder-Channel-Shield-Arduino-Raspberry/dp/B00E0NSORY/ref=sr_1_1?crid=1019L5X3H67SA&amp;dib=eyJ2IjoiMSJ9.cRdM_hhixgwOwN4y311Ism-JcvKPwbDObG3jxZWNAznpppkoNUWPD_aMk1Xa0q75KrqbyfL0LbLwwZ4ItCdcrV6zgJ83NVP7c-GHAPattiQDQXffcSqVTbAshK-ZoG2JDMXPV9b-qS1JjwHg2Tt4SU6vOT2NZpltCc7qu6IunR6hzjCDAQ7s33MMUFSbA4tF2-iibtlDr-h72Bpvoo4H9bDH4-0fqNBszXXFGS9WI_P12oaNx_DQeLHMm21uO3LyXOnHZROfyEWdJx2hA57EWYJG5FxhGbuIpe4klwDt53U.KHWy_-9JiCqYSpQpu-iTibBML1oHuQd-3NHI1G3J4uo&amp;dib_tag=se&amp;keywords=ELEGOO%2B4%2BChannel%2Brelay&amp;qid=1732572643&amp;s=industrial&amp;sprefix=elegoo%2B4%2Bchannel%2Brelay%2Cindustrial%2C92&amp;sr=1-1&amp;th=1</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/StarTech-com-USBAB1MR-Right-Angle-Cable/dp/B00FP32HI0/</t>
   </si>
 </sst>
 </file>
@@ -365,7 +339,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -403,6 +377,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -543,7 +523,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -553,11 +533,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="2" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
@@ -594,9 +573,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -634,7 +613,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -740,7 +719,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -882,7 +861,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -890,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FB30D09-70ED-6E46-895F-ABAD0978A38E}">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -902,868 +881,772 @@
     <col min="2" max="2" width="40.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.83203125" customWidth="1"/>
-    <col min="6" max="7" width="10.83203125" style="17"/>
+    <col min="6" max="6" width="11.5" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="11"/>
       <c r="B1" s="1" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="G1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F2" s="14"/>
+      <c r="G2" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>9</v>
+        <v>92</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3" s="17">
-        <v>9.58</v>
-      </c>
-      <c r="G3" s="18">
+      <c r="F3" s="16">
+        <v>44.54</v>
+      </c>
+      <c r="G3" s="17">
         <f>F3*E3</f>
-        <v>9.58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>44.54</v>
+      </c>
+      <c r="H3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>12.59</v>
       </c>
-      <c r="G4" s="18">
-        <f t="shared" ref="G4:G28" si="0">F4*E4</f>
+      <c r="G4" s="17">
+        <f t="shared" ref="G4:G27" si="0">F4*E4</f>
         <v>12.59</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>15</v>
+        <v>93</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" s="17">
-        <v>8.99</v>
-      </c>
-      <c r="G5" s="18">
+      <c r="F5" s="16">
+        <v>12.99</v>
+      </c>
+      <c r="G5" s="17">
         <f t="shared" si="0"/>
-        <v>8.99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>12.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C6" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" s="17">
-        <v>12.99</v>
-      </c>
-      <c r="G6" s="18">
+      <c r="F6" s="16">
+        <v>20.239999999999998</v>
+      </c>
+      <c r="G6" s="17">
         <f t="shared" si="0"/>
-        <v>12.99</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20.239999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>35</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>4.49</v>
+      </c>
+      <c r="G8" s="17">
+        <f t="shared" si="0"/>
+        <v>4.49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>10.59</v>
+      </c>
+      <c r="G9" s="17">
+        <f t="shared" si="0"/>
+        <v>10.59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D10" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" s="17">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>19.989999999999998</v>
+      </c>
+      <c r="G10" s="17">
+        <f t="shared" si="0"/>
+        <v>19.989999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="2"/>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16">
+        <v>488.4</v>
+      </c>
+      <c r="G11" s="17">
+        <f t="shared" si="0"/>
+        <v>488.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="2"/>
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="G12" s="17">
+        <f t="shared" si="0"/>
+        <v>18.399999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16">
+        <v>84.99</v>
+      </c>
+      <c r="G13" s="17">
+        <f t="shared" si="0"/>
+        <v>84.99</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="2"/>
+      <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
         <v>7.99</v>
       </c>
-      <c r="G8" s="18">
+      <c r="G14" s="17">
         <f t="shared" si="0"/>
         <v>7.99</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="17">
-        <v>16.989999999999998</v>
-      </c>
-      <c r="G9" s="18">
-        <f t="shared" si="0"/>
-        <v>16.989999999999998</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="17">
-        <v>27.99</v>
-      </c>
-      <c r="G10" s="18">
-        <f t="shared" si="0"/>
-        <v>27.99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
-      <c r="B11" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" s="17">
-        <v>498.61</v>
-      </c>
-      <c r="G11" s="18">
-        <f t="shared" si="0"/>
-        <v>498.61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="2"/>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="17">
-        <v>49.97</v>
-      </c>
-      <c r="G12" s="18">
-        <f t="shared" si="0"/>
-        <v>49.97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="2"/>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="17">
-        <v>7.99</v>
-      </c>
-      <c r="G13" s="18">
-        <f t="shared" si="0"/>
-        <v>7.99</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="2"/>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="G14" s="18">
-        <f t="shared" si="0"/>
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="2"/>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="E15">
         <v>1</v>
       </c>
-      <c r="F15" s="17">
-        <v>5.99</v>
-      </c>
-      <c r="G15" s="18">
+      <c r="F15" s="16">
+        <v>2.95</v>
+      </c>
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
-        <v>5.99</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+        <v>2.95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="2"/>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>43</v>
+        <v>97</v>
       </c>
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16" s="17">
-        <v>9.9600000000000009</v>
-      </c>
-      <c r="G16" s="18">
+      <c r="F16" s="16">
+        <v>10.99</v>
+      </c>
+      <c r="G16" s="17">
         <f t="shared" si="0"/>
-        <v>9.9600000000000009</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+        <v>10.99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="E17">
         <v>1</v>
       </c>
-      <c r="F17" s="17">
-        <v>15.95</v>
-      </c>
-      <c r="G17" s="18">
+      <c r="F17" s="16">
+        <v>18.98</v>
+      </c>
+      <c r="G17" s="17">
         <f t="shared" si="0"/>
-        <v>15.95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+        <v>18.98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="2"/>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>72</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
-      <c r="F18" s="17">
-        <v>2.77</v>
-      </c>
-      <c r="G18" s="18">
+      <c r="F18" s="16">
+        <v>7.36</v>
+      </c>
+      <c r="G18" s="17">
         <f t="shared" si="0"/>
-        <v>5.54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+        <v>14.72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="2"/>
       <c r="B19" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19" s="17">
-        <v>28.12</v>
-      </c>
-      <c r="G19" s="18">
+      <c r="F19" s="16">
+        <v>33.479999999999997</v>
+      </c>
+      <c r="G19" s="17">
         <f>E19*F19</f>
-        <v>28.12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+        <v>33.479999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="2"/>
       <c r="B20" s="5" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="E20">
         <v>3</v>
       </c>
-      <c r="F20" s="17">
-        <v>28.69</v>
-      </c>
-      <c r="G20" s="18">
-        <f t="shared" ref="G20:G24" si="1">E20*F20</f>
-        <v>86.070000000000007</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F20" s="16">
+        <v>33.04</v>
+      </c>
+      <c r="G20" s="17">
+        <f t="shared" ref="G20:G23" si="1">E20*F20</f>
+        <v>99.12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="2"/>
       <c r="B21" s="5" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="17">
-        <v>31.86</v>
-      </c>
-      <c r="G21" s="18">
+      <c r="F21" s="16">
+        <v>37.93</v>
+      </c>
+      <c r="G21" s="17">
         <f t="shared" si="1"/>
-        <v>63.72</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+        <v>75.86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="2"/>
       <c r="B22" s="5" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="C22" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="16">
         <v>67</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22" s="17">
-        <v>56.29</v>
-      </c>
-      <c r="G22" s="18">
+      <c r="G22" s="17">
         <f t="shared" si="1"/>
-        <v>56.29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="B23" s="5" t="s">
-        <v>68</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="E23">
         <v>1</v>
       </c>
-      <c r="F23" s="17">
-        <v>35.14</v>
-      </c>
-      <c r="G23" s="18">
+      <c r="F23" s="16">
+        <v>40.5</v>
+      </c>
+      <c r="G23" s="17">
         <f t="shared" si="1"/>
-        <v>35.14</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+        <v>40.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="2"/>
-      <c r="B24" s="5" t="s">
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="F24" s="16">
+        <v>14.2</v>
+      </c>
+      <c r="G24" s="17">
+        <f t="shared" ref="G24" si="2">F24*E24</f>
+        <v>56.8</v>
+      </c>
+      <c r="H24" t="s">
         <v>73</v>
       </c>
-      <c r="C24" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24" s="17">
-        <v>63.71</v>
-      </c>
-      <c r="G24" s="18">
-        <f t="shared" si="1"/>
-        <v>63.71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="2"/>
       <c r="B25" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="C25" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="E25">
-        <v>2</v>
-      </c>
-      <c r="F25" s="17">
-        <v>14.2</v>
-      </c>
-      <c r="G25" s="18">
-        <f t="shared" ref="G25" si="2">F25*E25</f>
-        <v>28.4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="F25" s="16">
+        <v>27.37</v>
+      </c>
+      <c r="G25" s="17">
+        <f t="shared" si="0"/>
+        <v>27.37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="2"/>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="C26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>84</v>
+        <v>63</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>64</v>
       </c>
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26" s="17">
-        <v>24.18</v>
-      </c>
-      <c r="G26" s="18">
+      <c r="F26" s="16">
+        <v>183.95</v>
+      </c>
+      <c r="G26" s="17">
         <f t="shared" si="0"/>
-        <v>24.18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+        <v>183.95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="2"/>
       <c r="B27" t="s">
-        <v>86</v>
-      </c>
-      <c r="C27" t="s">
-        <v>87</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27" s="17">
-        <v>129.94999999999999</v>
-      </c>
-      <c r="G27" s="18">
+      <c r="F27" s="18">
+        <v>50</v>
+      </c>
+      <c r="G27" s="17">
         <f t="shared" si="0"/>
-        <v>129.94999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13">
-        <v>1</v>
-      </c>
-      <c r="F28" s="19">
-        <v>15</v>
-      </c>
-      <c r="G28" s="18">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29" s="10"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="20"/>
-      <c r="G29" s="21"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" s="2"/>
-      <c r="B30" t="s">
-        <v>94</v>
-      </c>
-      <c r="C30" t="s">
-        <v>92</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="E30">
-        <v>1</v>
-      </c>
-      <c r="F30" s="17">
-        <v>695</v>
-      </c>
-      <c r="G30" s="18">
-        <f>E30*F30</f>
-        <v>695</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="10"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C29" t="s">
+        <v>82</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29" s="16">
+        <v>83.38</v>
+      </c>
+      <c r="G29" s="17">
+        <f t="shared" ref="G29" si="3">E29*F29</f>
+        <v>83.38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="10"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
-      <c r="B31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C31" t="s">
-        <v>95</v>
+      <c r="B31" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>43</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>96</v>
+        <v>44</v>
       </c>
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31" s="17">
-        <v>558</v>
-      </c>
-      <c r="G31" s="18">
-        <f t="shared" ref="G31:G33" si="3">E31*F31</f>
-        <v>558</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F31" s="16">
+        <v>35.74</v>
+      </c>
+      <c r="G31" s="17">
+        <f>E31*F31</f>
+        <v>35.74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="2"/>
-      <c r="B32" t="s">
-        <v>105</v>
+      <c r="B32" s="5" t="s">
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>97</v>
+        <v>49</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>98</v>
+        <v>50</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32" s="17">
-        <v>8.56</v>
-      </c>
-      <c r="G32" s="18">
-        <f t="shared" si="3"/>
-        <v>8.56</v>
+        <v>2</v>
+      </c>
+      <c r="F32" s="16">
+        <v>40.6</v>
+      </c>
+      <c r="G32" s="17">
+        <f>E32*F32</f>
+        <v>81.2</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2"/>
       <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="E33">
         <v>1</v>
       </c>
-      <c r="F33" s="17">
-        <v>56.29</v>
-      </c>
-      <c r="G33" s="18">
-        <f t="shared" si="3"/>
-        <v>56.29</v>
+      <c r="F33" s="16">
+        <v>142.41999999999999</v>
+      </c>
+      <c r="G33" s="17">
+        <f>E33*F33</f>
+        <v>142.41999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="2"/>
-      <c r="B34" t="s">
-        <v>101</v>
-      </c>
-      <c r="C34" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34" s="17">
-        <f>3480-SUM(F30:F33)</f>
-        <v>2162.15</v>
-      </c>
-      <c r="G34" s="18">
+      <c r="A34" s="7"/>
+      <c r="B34" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="8">
+        <v>1</v>
+      </c>
+      <c r="F34" s="21">
+        <v>36.97</v>
+      </c>
+      <c r="G34" s="22">
         <f>E34*F34</f>
-        <v>2162.15</v>
+        <v>36.97</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="21"/>
+      <c r="D35" s="3"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" s="2"/>
-      <c r="B36" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36" s="17">
-        <v>33.4</v>
-      </c>
-      <c r="G36" s="18">
-        <f>E36*F36</f>
-        <v>33.4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" s="2"/>
-      <c r="B37" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E37">
-        <v>2</v>
-      </c>
-      <c r="F37" s="17">
-        <v>37.94</v>
-      </c>
-      <c r="G37" s="18">
-        <f>E37*F37</f>
-        <v>75.88</v>
-      </c>
+      <c r="B36" s="5"/>
+      <c r="D36" s="3"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" s="2"/>
-      <c r="B38" s="5" t="s">
-        <v>102</v>
-      </c>
-      <c r="C38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38" s="17">
-        <v>112.56</v>
-      </c>
-      <c r="G38" s="18">
-        <f>E38*F38</f>
-        <v>112.56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" s="7"/>
-      <c r="B39" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E39" s="8">
-        <v>1</v>
-      </c>
-      <c r="F39" s="22">
-        <v>24.87</v>
-      </c>
-      <c r="G39" s="23">
-        <f>E39*F39</f>
-        <v>24.87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="F41" s="17" t="s">
-        <v>103</v>
-      </c>
-      <c r="G41" s="17">
-        <f>SUM(G3:G39)</f>
-        <v>4984.37</v>
+      <c r="F38" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G38" s="16">
+        <f>SUM(G3:G34)</f>
+        <v>1821.64</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D4" r:id="rId1" xr:uid="{57DDAFDF-7F9E-6440-BD35-A95D5616A2B9}"/>
-    <hyperlink ref="D14" r:id="rId2" xr:uid="{49D6F73C-EF77-B540-8EB5-138D28757B1F}"/>
-    <hyperlink ref="D27" r:id="rId3" xr:uid="{AB7AC4F4-7224-BB46-AAC2-4E2E21FDEE61}"/>
+    <hyperlink ref="D15" r:id="rId2" xr:uid="{49D6F73C-EF77-B540-8EB5-138D28757B1F}"/>
+    <hyperlink ref="D26" r:id="rId3" xr:uid="{AB7AC4F4-7224-BB46-AAC2-4E2E21FDEE61}"/>
     <hyperlink ref="D18" r:id="rId4" xr:uid="{8280B5C2-B78F-B741-ABFF-8FAF7BCC784C}"/>
-    <hyperlink ref="D16" r:id="rId5" xr:uid="{841BC566-163F-6F4C-8C39-C44140FB2548}"/>
-    <hyperlink ref="D13" r:id="rId6" xr:uid="{B0700279-B3E1-AD42-BD61-6A9DB4241F99}"/>
-    <hyperlink ref="D12" r:id="rId7" xr:uid="{4920C7D1-854E-5F44-B3E1-C68C08A626C2}"/>
+    <hyperlink ref="D17" r:id="rId5" xr:uid="{841BC566-163F-6F4C-8C39-C44140FB2548}"/>
+    <hyperlink ref="D14" r:id="rId6" display="https://www.amazon.com/ELEGOO-Channel-Optocoupler-Compatible-Raspberry/dp/B09ZQS2JRD/" xr:uid="{B0700279-B3E1-AD42-BD61-6A9DB4241F99}"/>
+    <hyperlink ref="D13" r:id="rId7" xr:uid="{4920C7D1-854E-5F44-B3E1-C68C08A626C2}"/>
     <hyperlink ref="D9" r:id="rId8" xr:uid="{ED56928F-6A8A-AB43-ABF6-47E78D70B6DC}"/>
     <hyperlink ref="D5" r:id="rId9" xr:uid="{78E8283F-A329-A144-907B-DD10D3A4D0DE}"/>
     <hyperlink ref="D10" r:id="rId10" xr:uid="{52D2E8FD-450D-0A4F-9C7B-5A1CF4DBB6F0}"/>
     <hyperlink ref="D21" r:id="rId11" xr:uid="{520D56F7-3B23-8049-8282-B0231B0FA5B1}"/>
-    <hyperlink ref="D19" r:id="rId12" xr:uid="{8D31C4F3-E750-E446-9E98-EE60D05362F7}"/>
-    <hyperlink ref="D20" r:id="rId13" xr:uid="{BFCB9E87-C449-CC49-88B4-11AE13DFB2AF}"/>
-    <hyperlink ref="D22" r:id="rId14" xr:uid="{070BF7CA-0CCC-0B46-A7EF-A1AA789E1CF4}"/>
-    <hyperlink ref="D23" r:id="rId15" xr:uid="{A53F6D01-ECEF-304A-B8A4-0D782AD1BFE9}"/>
-    <hyperlink ref="D36" r:id="rId16" xr:uid="{E6F65E80-EE12-5B4D-A244-B52CF85E914D}"/>
-    <hyperlink ref="D37" r:id="rId17" xr:uid="{68FFC1F0-0B13-914A-AD30-89C331E0F1D2}"/>
-    <hyperlink ref="D26" r:id="rId18" xr:uid="{0C39E4C2-B5A8-D040-AB35-4BEC472A5DDF}"/>
-    <hyperlink ref="D3" r:id="rId19" xr:uid="{D4EC7B19-5C71-FD47-978B-1323B2D0E6AF}"/>
-    <hyperlink ref="D6" r:id="rId20" xr:uid="{CF1EF7D8-6FFE-E54D-B22B-6F2D97C25624}"/>
-    <hyperlink ref="D7" r:id="rId21" xr:uid="{47187895-7F78-3345-8613-4DF59DA82653}"/>
-    <hyperlink ref="D8" r:id="rId22" xr:uid="{83FF4F88-180B-F749-9AAB-D87B590F5768}"/>
-    <hyperlink ref="D11" r:id="rId23" xr:uid="{008EF63E-9AA4-FD45-867B-5AFB664FD164}"/>
-    <hyperlink ref="D15" r:id="rId24" xr:uid="{16109325-2214-1241-9FE8-12B6F234B7DF}"/>
-    <hyperlink ref="D17" r:id="rId25" xr:uid="{2C5C76F9-503B-804B-8187-CF21D02503CB}"/>
-    <hyperlink ref="D38" r:id="rId26" xr:uid="{1EC09A48-D24F-F543-9D49-41E0A7623ECF}"/>
-    <hyperlink ref="D24" r:id="rId27" xr:uid="{49EFB861-5AFD-3C49-9D8C-5002E7AC9BC7}"/>
-    <hyperlink ref="D39" r:id="rId28" xr:uid="{08DA4DC3-770E-2643-92E6-9637E1065D43}"/>
-    <hyperlink ref="D25" r:id="rId29" xr:uid="{F8A36783-ECE3-4E44-BEC4-62C600C8B298}"/>
-    <hyperlink ref="D31" r:id="rId30" xr:uid="{63B18B15-B998-CD4F-BF8A-77D78A7812CF}"/>
-    <hyperlink ref="D32" r:id="rId31" xr:uid="{07BB656F-215D-4D4B-9F02-B1BB22A78A29}"/>
-    <hyperlink ref="D33" r:id="rId32" xr:uid="{24EB6D9A-4514-E341-AB4B-A62D3EAD6F71}"/>
-    <hyperlink ref="D30" r:id="rId33" xr:uid="{783E9EA8-964D-3042-9989-BB5925D36400}"/>
+    <hyperlink ref="D20" r:id="rId12" xr:uid="{BFCB9E87-C449-CC49-88B4-11AE13DFB2AF}"/>
+    <hyperlink ref="D31" r:id="rId13" xr:uid="{E6F65E80-EE12-5B4D-A244-B52CF85E914D}"/>
+    <hyperlink ref="D32" r:id="rId14" xr:uid="{68FFC1F0-0B13-914A-AD30-89C331E0F1D2}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{0C39E4C2-B5A8-D040-AB35-4BEC472A5DDF}"/>
+    <hyperlink ref="D3" r:id="rId16" display="https://www.digikey.com/en/products/detail/traco-power/TMPW%252050-112-T/20525617?gclsrc=aw.ds&amp;&amp;utm_adgroup=&amp;utm_source=google&amp;utm_medium=cpc&amp;utm_campaign=Pmax_Shopping_DK%2B%20Supplier_ITECH&amp;utm_term=&amp;utm_content=&amp;utm_id=go_cmp-21147141757_adg-_ad-__dev-c_ext-_prd-20525617_sig-CjwKCAiA3ZC6BhBaEiwAeqfvyjKG0U8PWJcrc_QQsXyUxfll2yvNX7vfMULlS1uMNy8c9vlZJXY1VxoCGvoQAvD_BwE&amp;gad_source=1&amp;gbraid=0AAAAADrbLljvEBu8WsSuhejydM0PsvfLA&amp;gclid=CjwKCAiA3ZC6BhBaEiwAeqfvyjKG0U8PWJcrc_QQsXyUxfll2yvNX7vfMULlS1uMNy8c9vlZJXY1VxoCGvoQAvD_BwE&amp;gclsrc=aw.ds" xr:uid="{D4EC7B19-5C71-FD47-978B-1323B2D0E6AF}"/>
+    <hyperlink ref="D6" r:id="rId17" xr:uid="{CF1EF7D8-6FFE-E54D-B22B-6F2D97C25624}"/>
+    <hyperlink ref="D8" r:id="rId18" xr:uid="{83FF4F88-180B-F749-9AAB-D87B590F5768}"/>
+    <hyperlink ref="D11" r:id="rId19" xr:uid="{008EF63E-9AA4-FD45-867B-5AFB664FD164}"/>
+    <hyperlink ref="D16" r:id="rId20" xr:uid="{16109325-2214-1241-9FE8-12B6F234B7DF}"/>
+    <hyperlink ref="D33" r:id="rId21" xr:uid="{1EC09A48-D24F-F543-9D49-41E0A7623ECF}"/>
+    <hyperlink ref="D34" r:id="rId22" xr:uid="{08DA4DC3-770E-2643-92E6-9637E1065D43}"/>
+    <hyperlink ref="D24" r:id="rId23" xr:uid="{F8A36783-ECE3-4E44-BEC4-62C600C8B298}"/>
+    <hyperlink ref="D19" r:id="rId24" xr:uid="{8D31C4F3-E750-E446-9E98-EE60D05362F7}"/>
+    <hyperlink ref="D29" r:id="rId25" xr:uid="{24EB6D9A-4514-E341-AB4B-A62D3EAD6F71}"/>
+    <hyperlink ref="D22" r:id="rId26" xr:uid="{D1E123BB-BF31-0C43-B47F-1CFAAAB1BFBF}"/>
+    <hyperlink ref="D12" r:id="rId27" xr:uid="{E4F72412-391C-8D4B-AC79-A10C5FD11557}"/>
+    <hyperlink ref="D23" r:id="rId28" xr:uid="{079F5545-8635-B84D-8A9D-DF6122334C80}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>